<commit_message>
a suti oldal szekesztése
</commit_message>
<xml_diff>
--- a/Lucky_cafe/.egyebek/sutemenyek-kaloria-tablazat.xlsx
+++ b/Lucky_cafe/.egyebek/sutemenyek-kaloria-tablazat.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KerteszBarnabas\OneDrive - BGéSZC Katona József Technikum\Asztal\Github\Lucky_cafe_project\Lucky_cafe\.egyebek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sulis\Desktop\github\Lucky_cafe_project\Lucky_cafe\.egyebek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4D6204247ACDAA4110B4902957F328693EDF15" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{AB657FB3-ABED-498C-B485-5612872F2662}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647899CC-945B-4CD7-B9BE-733F0D2A6CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="sütemények" sheetId="1" r:id="rId1"/>
+    <sheet name="kávék" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,8 +25,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1A244E31-7C3E-4B09-ADEF-676762605900}</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1A244E31-7C3E-4B09-ADEF-676762605900}">
+      <text>
+        <t>[Témakörökbe rendezett megjegyzés]
+Ebben az Excel-verzióban olvasni tudja ezt a témakörökbe rendezett megjegyzést, ha viszont újabb Excel-verzióban nyitja meg a fájlt, eltávolítjuk a módosításait a megjegyzésből. További információ: https://go.microsoft.com/fwlink/?linkid=870924
+Megjegyzés:
+    Maga a kávé mekkora?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Áfonya torta</t>
   </si>
@@ -73,19 +92,46 @@
   </si>
   <si>
     <t>476 Kcal</t>
+  </si>
+  <si>
+    <t>név</t>
+  </si>
+  <si>
+    <t>kép</t>
+  </si>
+  <si>
+    <t>kávé</t>
+  </si>
+  <si>
+    <t>víz/tej</t>
+  </si>
+  <si>
+    <t>tejszín</t>
+  </si>
+  <si>
+    <t>alkotás</t>
+  </si>
+  <si>
+    <t>mekkora?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,6 +171,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Eberling Ferenc Tamas" id="{FFD13443-C9FC-4F03-92C5-CD719621EE2E}" userId="S::ferenctamas.eberling@katonaj-mkszig.hu::7709d254-1d55-4cec-8067-58e733573893" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,11 +440,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2023-01-14T10:31:14.48" personId="{FFD13443-C9FC-4F03-92C5-CD719621EE2E}" id="{1A244E31-7C3E-4B09-ADEF-676762605900}">
+    <text>Maga a kávé mekkora?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -470,4 +530,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F949C-605A-4B21-87AA-AC036911E2EE}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>